<commit_message>
added parts needed for BOM + parts from other HotWire hardware ( maintained by different user)
</commit_message>
<xml_diff>
--- a/Hardware/HotWireADC/Rev2/BOMHotWireRev2.xlsx
+++ b/Hardware/HotWireADC/Rev2/BOMHotWireRev2.xlsx
@@ -18,12 +18,12 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">HotWireRev2!$B$2:$B$49</definedName>
     <definedName name="_xlnm.Extract" localSheetId="0">HotWireRev2!$G$4</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="158">
   <si>
     <t>Reference</t>
   </si>
@@ -278,13 +278,232 @@
   </si>
   <si>
     <t>P6</t>
+  </si>
+  <si>
+    <t>Mouser Link</t>
+  </si>
+  <si>
+    <t>http://www.mouser.co.uk/Search/ProductDetail.aspx?R=ADS8331IPWvirtualkey59500000virtualkey595-ADS8331IPW</t>
+  </si>
+  <si>
+    <t>http://www.mouser.co.uk/Search/ProductDetail.aspx?R=OPA320AIDBVRvirtualkey59500000virtualkey595-OPA320AIDBVR</t>
+  </si>
+  <si>
+    <t>http://www.mouser.co.uk/Search/ProductDetail.aspx?R=VJ1206Y152KXXCW1BCvirtualkey61340000virtualkey77-VJ1206Y152KXXCBC</t>
+  </si>
+  <si>
+    <t>http://www.mouser.co.uk/Search/ProductDetail.aspx?R=L78S05CVvirtualkey51120000virtualkey511-L78S05CV</t>
+  </si>
+  <si>
+    <t>http://www.mouser.co.uk/Search/ProductDetail.aspx?R=RASM712Xvirtualkey50210000virtualkey502-RASM712X</t>
+  </si>
+  <si>
+    <t>http://www.mouser.co.uk/Search/ProductDetail.aspx?R=2-1437565-8virtualkey50660000virtualkey506-2-1437565-8</t>
+  </si>
+  <si>
+    <t>http://www.mouser.co.uk/Search/ProductDetail.aspx?R=12065A751JAT2Avirtualkey58110000virtualkey581-12065A751JAT2A</t>
+  </si>
+  <si>
+    <t>http://www.mouser.co.uk/Search/ProductDetail.aspx?R=VJ1206Y104KXBATvirtualkey61340000virtualkey77-VJ1206Y104KXBAT</t>
+  </si>
+  <si>
+    <t>http://www.mouser.co.uk/Search/ProductDetail.aspx?R=VJ1206Y105KXQTW1BCvirtualkey61340000virtualkey77-VJ1206Y105KXQTBC</t>
+  </si>
+  <si>
+    <t>http://www.mouser.co.uk/Search/ProductDetail.aspx?R=VJ1206V106ZXQTW1BCvirtualkey61340000virtualkey77-VJ1206V106ZXQTBC</t>
+  </si>
+  <si>
+    <t>http://www.mouser.co.uk/Search/ProductDetail.aspx?R=F931A106MAAvirtualkey58110000virtualkey647-F931A106MAA</t>
+  </si>
+  <si>
+    <t>http://www.mouser.co.uk/Search/ProductDetail.aspx?R=REF5040AIDRvirtualkey59500000virtualkey595-REF5040AIDR</t>
+  </si>
+  <si>
+    <t>http://www.mouser.co.uk/Search/ProductDetail.aspx?R=ERJ-8ENF34R8Vvirtualkey66720000virtualkey667-ERJ-8ENF34R8V</t>
+  </si>
+  <si>
+    <t>http://www.mouser.co.uk/Search/ProductDetail.aspx?R=RL1206FR-070R5Lvirtualkey60120000virtualkey603-RL1206FR070R5L</t>
+  </si>
+  <si>
+    <t>http://www.mouser.co.uk/Search/ProductDetail.aspx?R=CRCW120610K0FKEAvirtualkey61300000virtualkey71-CRCW1206-10K-E3</t>
+  </si>
+  <si>
+    <t>http://www.mouser.co.uk/Search/ProductDetail.aspx?R=5-1634503-1virtualkey57100000virtualkey571-5-1634503-1</t>
+  </si>
+  <si>
+    <t>595-ADS8331IPW</t>
+  </si>
+  <si>
+    <t>Mouser Part No</t>
+  </si>
+  <si>
+    <t>511-L78S05CV</t>
+  </si>
+  <si>
+    <t>647-F931A106MAA</t>
+  </si>
+  <si>
+    <t>502-RASM712X</t>
+  </si>
+  <si>
+    <t>77-VJ1206Y105KXQTBC</t>
+  </si>
+  <si>
+    <t>77-VJ1206V106ZXQTBC</t>
+  </si>
+  <si>
+    <t>77-VJ1206Y104KXBAT</t>
+  </si>
+  <si>
+    <t>77-VJ1206Y152KXXCBC</t>
+  </si>
+  <si>
+    <t>581-12065A751JAT2A</t>
+  </si>
+  <si>
+    <t>581-1206ZG226ZAT2A</t>
+  </si>
+  <si>
+    <t>22u</t>
+  </si>
+  <si>
+    <t>0.22Ohm</t>
+  </si>
+  <si>
+    <t>279-RL73K2BR22JTD</t>
+  </si>
+  <si>
+    <t>667-ERJ-8ENF34R8V</t>
+  </si>
+  <si>
+    <t>603-RL1206FR070R5L</t>
+  </si>
+  <si>
+    <t>595-OPA320AIDBVR</t>
+  </si>
+  <si>
+    <t>595-REF5040AIDR</t>
+  </si>
+  <si>
+    <t>571-5-1634503-1</t>
+  </si>
+  <si>
+    <t>Kostas BNC connector</t>
+  </si>
+  <si>
+    <t>571-1-1337543-0</t>
+  </si>
+  <si>
+    <t>506-2-1437565-8</t>
+  </si>
+  <si>
+    <t>100ohm</t>
+  </si>
+  <si>
+    <t>594-53611101</t>
+  </si>
+  <si>
+    <t>1k</t>
+  </si>
+  <si>
+    <t>858-P160KN0QD15B1K</t>
+  </si>
+  <si>
+    <t>20k</t>
+  </si>
+  <si>
+    <t>858-P160KN-0QC15B20K</t>
+  </si>
+  <si>
+    <t>knob for pot</t>
+  </si>
+  <si>
+    <t>652-H-22-6A</t>
+  </si>
+  <si>
+    <t>71-CRCW1206-10K-E3</t>
+  </si>
+  <si>
+    <t>Extra filter</t>
+  </si>
+  <si>
+    <t>470pf</t>
+  </si>
+  <si>
+    <t>150pf</t>
+  </si>
+  <si>
+    <t>LM555CN</t>
+  </si>
+  <si>
+    <t>4.7nF</t>
+  </si>
+  <si>
+    <t>Rapid part no</t>
+  </si>
+  <si>
+    <t>11-3438</t>
+  </si>
+  <si>
+    <t>11-3436</t>
+  </si>
+  <si>
+    <t>2.2nf</t>
+  </si>
+  <si>
+    <t>11-3409</t>
+  </si>
+  <si>
+    <t>11-3431</t>
+  </si>
+  <si>
+    <t>220pf</t>
+  </si>
+  <si>
+    <t>11-3433</t>
+  </si>
+  <si>
+    <t>512-LM555CN</t>
+  </si>
+  <si>
+    <t>http://www.mouser.co.uk/ProductDetail/Fairchild-Semiconductor/LM555CN/?qs=sGAEpiMZZMsFq5dYAzx%252bAD%2fV68CJyZkdR88eRK4OGz0%3d</t>
+  </si>
+  <si>
+    <t>http://www.mouser.co.uk/ProductDetail/TDK/FG18C0G1H222JNT06/?qs=sGAEpiMZZMsh%252b1woXyUXj2I8eAiqPMPDS9EODJDvjQc%3d</t>
+  </si>
+  <si>
+    <t>810-FG18C0G1H222JNT6</t>
+  </si>
+  <si>
+    <t>810-FG18C0G1H471JNT6</t>
+  </si>
+  <si>
+    <t>http://www.mouser.co.uk/ProductDetail/TDK/FG18C0G1H471JNT06/?qs=sGAEpiMZZMsh%252b1woXyUXj2I8eAiqPMPDZ0avY%2fssMCw%3d</t>
+  </si>
+  <si>
+    <t>810-FG18C0G1H221JNT6</t>
+  </si>
+  <si>
+    <t>http://www.mouser.co.uk/ProductDetail/TDK/FG18C0G1H221JNT06/?qs=sGAEpiMZZMsh%252b1woXyUXj2I8eAiqPMPDzPrTMNVSiEU%3d</t>
+  </si>
+  <si>
+    <t>810-FG18C0G1H151JNT0</t>
+  </si>
+  <si>
+    <t>http://www.mouser.co.uk/ProductDetail/TDK/FG18C0G1H151JNT00/?qs=sGAEpiMZZMsh%252b1woXyUXj8A36jb%2fuMHolhKiAmkqhAE%3d</t>
+  </si>
+  <si>
+    <t>810-FG18X7R1H472KNT0</t>
+  </si>
+  <si>
+    <t>http://www.mouser.co.uk/ProductDetail/TDK/FG18X7R1H472KNT00/?qs=sGAEpiMZZMsh%252b1woXyUXj8A36jb%2fuMHow1%2ff8sE6VsM%3d</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -419,6 +638,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -717,7 +952,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -760,11 +995,20 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -798,6 +1042,7 @@
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -1096,10 +1341,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H49"/>
+  <dimension ref="A1:J49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+    <sheetView tabSelected="1" topLeftCell="D13" workbookViewId="0">
+      <selection activeCell="M35" sqref="M35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1107,9 +1352,11 @@
     <col min="1" max="1" width="12.28515625" customWidth="1"/>
     <col min="3" max="3" width="63.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.5703125" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1123,7 +1370,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1134,7 +1381,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -1144,8 +1391,14 @@
       <c r="C3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I3" t="s">
+        <v>103</v>
+      </c>
+      <c r="J3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -1162,8 +1415,14 @@
         <f>COUNTIF($B$2:$B$49,G4)</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I4" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="J4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -1177,11 +1436,17 @@
         <v>11</v>
       </c>
       <c r="H5">
-        <f t="shared" ref="H4:H23" si="0">COUNTIF($B$2:$B$49,G5)</f>
+        <f t="shared" ref="H5:H15" si="0">COUNTIF($B$2:$B$49,G5)</f>
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I5" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="J5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -1198,8 +1463,12 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I6" t="e">
+        <f>----- 71-RN60D39R2FTR</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -1216,8 +1485,14 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I7" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="J7" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -1234,8 +1509,14 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I8" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="J8" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -1252,8 +1533,14 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I9" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="J9" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -1270,8 +1557,14 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I10" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="J10" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>23</v>
       </c>
@@ -1288,8 +1581,14 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I11" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="J11" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>24</v>
       </c>
@@ -1306,8 +1605,14 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I12" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="J12" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>25</v>
       </c>
@@ -1324,8 +1629,14 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I13" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="J13" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -1342,8 +1653,14 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I14" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>27</v>
       </c>
@@ -1360,8 +1677,14 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I15" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="J15" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>28</v>
       </c>
@@ -1378,8 +1701,14 @@
         <f>COUNTIF($B$2:$B$49,G16)</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I16" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="J16" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>30</v>
       </c>
@@ -1396,8 +1725,14 @@
         <f>COUNTIF($B$2:$B$49,G17)</f>
         <v>2</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I17" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="J17" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>31</v>
       </c>
@@ -1414,8 +1749,14 @@
         <f>COUNTIF($B$2:$B$49,G18)</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I18" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="J18" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>33</v>
       </c>
@@ -1432,8 +1773,14 @@
         <f>COUNTIF($B$2:$B$49,G19)</f>
         <v>5</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I19" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="J19" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>34</v>
       </c>
@@ -1450,8 +1797,14 @@
         <f>COUNTIF($B$2:$B$49,G20)</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I20" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="J20" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>37</v>
       </c>
@@ -1462,7 +1815,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>39</v>
       </c>
@@ -1473,7 +1826,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>40</v>
       </c>
@@ -1484,7 +1837,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>42</v>
       </c>
@@ -1494,8 +1847,11 @@
       <c r="C24" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G24" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>44</v>
       </c>
@@ -1505,8 +1861,17 @@
       <c r="C25" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G25" t="s">
+        <v>113</v>
+      </c>
+      <c r="H25">
+        <v>1</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>46</v>
       </c>
@@ -1516,8 +1881,17 @@
       <c r="C26" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G26" t="s">
+        <v>114</v>
+      </c>
+      <c r="H26">
+        <v>1</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>47</v>
       </c>
@@ -1528,7 +1902,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>48</v>
       </c>
@@ -1539,7 +1913,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>51</v>
       </c>
@@ -1549,8 +1923,14 @@
       <c r="C29" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G29" t="s">
+        <v>121</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>52</v>
       </c>
@@ -1561,7 +1941,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>53</v>
       </c>
@@ -1571,8 +1951,14 @@
       <c r="C31" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G31" t="s">
+        <v>124</v>
+      </c>
+      <c r="I31" s="2" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>54</v>
       </c>
@@ -1582,8 +1968,14 @@
       <c r="C32" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="G32" t="s">
+        <v>126</v>
+      </c>
+      <c r="I32" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>55</v>
       </c>
@@ -1593,8 +1985,14 @@
       <c r="C33" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="G33" t="s">
+        <v>128</v>
+      </c>
+      <c r="I33" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>57</v>
       </c>
@@ -1605,7 +2003,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>58</v>
       </c>
@@ -1615,8 +2013,14 @@
       <c r="C35" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="G35" t="s">
+        <v>130</v>
+      </c>
+      <c r="I35" s="2" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>61</v>
       </c>
@@ -1627,7 +2031,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>62</v>
       </c>
@@ -1637,8 +2041,11 @@
       <c r="C37" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F37" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>63</v>
       </c>
@@ -1648,8 +2055,20 @@
       <c r="C38" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F38" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="G38" t="s">
+        <v>137</v>
+      </c>
+      <c r="I38" t="s">
+        <v>156</v>
+      </c>
+      <c r="J38" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>65</v>
       </c>
@@ -1659,8 +2078,20 @@
       <c r="C39" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F39" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="G39" t="s">
+        <v>141</v>
+      </c>
+      <c r="I39" t="s">
+        <v>149</v>
+      </c>
+      <c r="J39" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>67</v>
       </c>
@@ -1670,8 +2101,20 @@
       <c r="C40" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F40" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="G40" t="s">
+        <v>134</v>
+      </c>
+      <c r="I40" t="s">
+        <v>150</v>
+      </c>
+      <c r="J40" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>68</v>
       </c>
@@ -1681,8 +2124,20 @@
       <c r="C41" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F41" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="G41" t="s">
+        <v>144</v>
+      </c>
+      <c r="I41" t="s">
+        <v>152</v>
+      </c>
+      <c r="J41" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>69</v>
       </c>
@@ -1692,8 +2147,20 @@
       <c r="C42" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F42" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="G42" t="s">
+        <v>135</v>
+      </c>
+      <c r="I42" t="s">
+        <v>154</v>
+      </c>
+      <c r="J42" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>72</v>
       </c>
@@ -1703,8 +2170,9 @@
       <c r="C43" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F43" s="4"/>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>75</v>
       </c>
@@ -1714,8 +2182,9 @@
       <c r="C44" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F44" s="4"/>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>76</v>
       </c>
@@ -1725,8 +2194,9 @@
       <c r="C45" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F45" s="4"/>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>77</v>
       </c>
@@ -1736,8 +2206,18 @@
       <c r="C46" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F46" s="4"/>
+      <c r="G46" t="s">
+        <v>136</v>
+      </c>
+      <c r="I46" t="s">
+        <v>146</v>
+      </c>
+      <c r="J46" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>78</v>
       </c>
@@ -1747,8 +2227,9 @@
       <c r="C47" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F47" s="4"/>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>81</v>
       </c>
@@ -1758,6 +2239,7 @@
       <c r="C48" t="s">
         <v>83</v>
       </c>
+      <c r="F48" s="4"/>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
@@ -1771,9 +2253,35 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="J14" r:id="rId1"/>
+    <hyperlink ref="I4" r:id="rId2" display="http://www.mouser.co.uk/Search/ProductDetail.aspx?R=ADS8331IPWvirtualkey59500000virtualkey595-ADS8331IPW"/>
+    <hyperlink ref="I18" r:id="rId3" display="http://www.mouser.co.uk/Search/ProductDetail.aspx?R=L78S05CVvirtualkey51120000virtualkey511-L78S05CV"/>
+    <hyperlink ref="I17" r:id="rId4" display="http://www.mouser.co.uk/Search/ProductDetail.aspx?R=F931A106MAAvirtualkey58110000virtualkey647-F931A106MAA"/>
+    <hyperlink ref="I20" r:id="rId5" display="http://www.mouser.co.uk/Search/ProductDetail.aspx?R=RASM712Xvirtualkey50210000virtualkey502-RASM712X"/>
+    <hyperlink ref="I13" r:id="rId6" display="http://www.mouser.co.uk/Search/ProductDetail.aspx?R=VJ1206Y105KXQTW1BCvirtualkey61340000virtualkey77-VJ1206Y105KXQTBC"/>
+    <hyperlink ref="I14" r:id="rId7" display="http://www.mouser.co.uk/Search/ProductDetail.aspx?R=VJ1206V106ZXQTW1BCvirtualkey61340000virtualkey77-VJ1206V106ZXQTBC"/>
+    <hyperlink ref="I12" r:id="rId8" display="http://www.mouser.co.uk/Search/ProductDetail.aspx?R=VJ1206Y104KXBATvirtualkey61340000virtualkey77-VJ1206Y104KXBAT"/>
+    <hyperlink ref="I7" r:id="rId9" display="http://www.mouser.co.uk/Search/ProductDetail.aspx?R=VJ1206Y152KXXCW1BCvirtualkey61340000virtualkey77-VJ1206Y152KXXCBC"/>
+    <hyperlink ref="I10" r:id="rId10" display="http://www.mouser.co.uk/Search/ProductDetail.aspx?R=12065A751JAT2Avirtualkey58110000virtualkey581-12065A751JAT2A"/>
+    <hyperlink ref="I25" r:id="rId11" display="http://www.mouser.co.uk/Search/ProductDetail.aspx?R=1206ZG226ZAT2Avirtualkey58110000virtualkey581-1206ZG226ZAT2A"/>
+    <hyperlink ref="I26" r:id="rId12" display="http://www.mouser.co.uk/Search/ProductDetail.aspx?R=RL73K2BR22JTDvirtualkey20420000virtualkey279-RL73K2BR22JTD"/>
+    <hyperlink ref="I9" r:id="rId13" display="http://www.mouser.co.uk/Search/ProductDetail.aspx?R=ERJ-8ENF34R8Vvirtualkey66720000virtualkey667-ERJ-8ENF34R8V"/>
+    <hyperlink ref="I15" r:id="rId14" display="http://www.mouser.co.uk/Search/ProductDetail.aspx?R=RL1206FR-070R5Lvirtualkey60120000virtualkey603-RL1206FR070R5L"/>
+    <hyperlink ref="I5" r:id="rId15" display="http://www.mouser.co.uk/Search/ProductDetail.aspx?R=OPA320AIDBVRvirtualkey59500000virtualkey595-OPA320AIDBVR"/>
+    <hyperlink ref="I16" r:id="rId16" display="http://www.mouser.co.uk/Search/ProductDetail.aspx?R=REF5040AIDRvirtualkey59500000virtualkey595-REF5040AIDR"/>
+    <hyperlink ref="I19" r:id="rId17" display="http://www.mouser.co.uk/Search/ProductDetail.aspx?R=5-1634503-1virtualkey57100000virtualkey571-5-1634503-1"/>
+    <hyperlink ref="I29" r:id="rId18" display="http://www.mouser.co.uk/Search/ProductDetail.aspx?R=1-1337543-0virtualkey57100000virtualkey571-1-1337543-0"/>
+    <hyperlink ref="I11" r:id="rId19" display="http://www.mouser.co.uk/Search/ProductDetail.aspx?R=2-1437565-8virtualkey50660000virtualkey506-2-1437565-8"/>
+    <hyperlink ref="I31" r:id="rId20" display="http://www.mouser.co.uk/Search/ProductDetail.aspx?R=536B101virtualkey59400000virtualkey594-53611101"/>
+    <hyperlink ref="I32" r:id="rId21" display="http://www.mouser.co.uk/Search/ProductDetail.aspx?R=P160KN-0QD15B1Kvirtualkey57700000virtualkey858-P160KN0QD15B1K"/>
+    <hyperlink ref="I33" r:id="rId22" display="http://www.mouser.co.uk/Search/ProductDetail.aspx?R=P160KN-0QC15B20Kvirtualkey57700000virtualkey858-P160KN-0QC15B20K"/>
+    <hyperlink ref="I35" r:id="rId23" display="http://www.mouser.co.uk/Search/ProductDetail.aspx?R=H-22-6Avirtualkey65210000virtualkey652-H-22-6A"/>
+    <hyperlink ref="I8" r:id="rId24" display="http://www.mouser.co.uk/Search/ProductDetail.aspx?R=CRCW120610K0FKEAvirtualkey61300000virtualkey71-CRCW1206-10K-E3"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId25"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>